<commit_message>
update my 2021 plan
</commit_message>
<xml_diff>
--- a/Personal/MillerToDoList.xlsx
+++ b/Personal/MillerToDoList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20370"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\notes\Personal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B5E381-AC20-4BB5-9B88-C610388E598B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6764F0-9AC2-42C0-86A0-1386C99CDFCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17535" activeTab="1" xr2:uid="{FBB7AB9A-5833-4D53-A287-E17DA39A5383}"/>
   </bookViews>
@@ -122,6 +122,85 @@
         </r>
       </text>
     </comment>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{F9B9F7B3-E2F5-41B3-BE9F-766D28D54F46}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>单东东:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+SpringBoot、Spring原理、深入理解Java虚拟机、Kafka</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{C72E3AB1-007F-491D-B7B2-BE9DCE9D7146}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>单东东:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+Jmeter系列文章
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{780EC25F-AA93-4193-A3EF-87D13F4FA479}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>单东东:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+Jenkins、Docker、凤凰项目、用户故事实战、DevOps实战指南</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -164,7 +243,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="197">
   <si>
     <t>周</t>
   </si>
@@ -479,276 +558,363 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>A课程-18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Java多线程Demo编写</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A课程-22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HTML、JavaScript复习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vue2入门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作习得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>尚硅谷VUE核心技术视频</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A课程-38</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逻辑英语系统4班180天</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C课程-38</t>
+  </si>
+  <si>
+    <t>C课程-40</t>
+  </si>
+  <si>
+    <t>E课程-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E课程-08</t>
+  </si>
+  <si>
+    <t>E课程-10</t>
+  </si>
+  <si>
+    <t>E课程-04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E课程-12</t>
+  </si>
+  <si>
+    <t>E课程-14</t>
+  </si>
+  <si>
+    <t>E课程-16</t>
+  </si>
+  <si>
+    <t>E课程-18</t>
+  </si>
+  <si>
+    <t>E课程-20</t>
+  </si>
+  <si>
+    <t>E课程-22</t>
+  </si>
+  <si>
+    <t>E课程-24</t>
+  </si>
+  <si>
+    <t>E课程-26</t>
+  </si>
+  <si>
+    <t>E课程-28</t>
+  </si>
+  <si>
+    <t>E课程-30</t>
+  </si>
+  <si>
+    <t>E课程-32</t>
+  </si>
+  <si>
+    <t>E课程-34</t>
+  </si>
+  <si>
+    <t>E课程-36</t>
+  </si>
+  <si>
+    <t>E课程-38</t>
+  </si>
+  <si>
+    <t>E课程-40</t>
+  </si>
+  <si>
+    <t>D课程-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D课程-04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D课程-06</t>
+  </si>
+  <si>
+    <t>D课程-08</t>
+  </si>
+  <si>
+    <t>D课程-10</t>
+  </si>
+  <si>
+    <t>D课程-12</t>
+  </si>
+  <si>
+    <t>D课程-14</t>
+  </si>
+  <si>
+    <t>D课程-16</t>
+  </si>
+  <si>
+    <t>D课程-18</t>
+  </si>
+  <si>
+    <t>D课程-20</t>
+  </si>
+  <si>
+    <t>D课程-22</t>
+  </si>
+  <si>
+    <t>D课程-24</t>
+  </si>
+  <si>
+    <t>D课程-26</t>
+  </si>
+  <si>
+    <t>D课程-28</t>
+  </si>
+  <si>
+    <t>D课程-30</t>
+  </si>
+  <si>
+    <t>D课程-32</t>
+  </si>
+  <si>
+    <t>D课程-34</t>
+  </si>
+  <si>
+    <t>D课程-36</t>
+  </si>
+  <si>
+    <t>D课程-38</t>
+  </si>
+  <si>
+    <t>D课程-40</t>
+  </si>
+  <si>
+    <t>B课程-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B课程-06</t>
+  </si>
+  <si>
+    <t>B课程-04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B课程-08</t>
+  </si>
+  <si>
+    <t>B课程-10</t>
+  </si>
+  <si>
+    <t>B课程-12</t>
+  </si>
+  <si>
+    <t>春节放假</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B课程-14</t>
+  </si>
+  <si>
+    <t>B课程-16</t>
+  </si>
+  <si>
+    <t>B课程-18</t>
+  </si>
+  <si>
+    <t>B课程-20</t>
+  </si>
+  <si>
+    <t>B课程-22</t>
+  </si>
+  <si>
+    <t>B课程-24</t>
+  </si>
+  <si>
+    <t>B课程-26</t>
+  </si>
+  <si>
+    <t>B课程-28</t>
+  </si>
+  <si>
+    <t>B课程-30</t>
+  </si>
+  <si>
+    <t>B课程-32</t>
+  </si>
+  <si>
+    <t>B课程-34</t>
+  </si>
+  <si>
+    <t>B课程-36</t>
+  </si>
+  <si>
+    <t>B课程-38</t>
+  </si>
+  <si>
+    <t>B课程-40</t>
+  </si>
+  <si>
+    <t>C课程-14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C课程-05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TypeScript入门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C课程-06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>性能测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E课程-06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逻辑英语系统4班360天</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vue开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务端开发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestOPS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miller笔记——Jmeter(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miller笔记——Jmeter(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miller笔记——Jmeter(3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miller笔记——Jmeter(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>213_尚硅谷Docker核心技术</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spring原理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>SpringBoot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Spring原理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>深入理解Java虚拟机</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>A课程-18</t>
+    <t>凤凰项目-P70</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Java多线程Demo编写</t>
+    <t>Jmeter性能测试实战-P70</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>A课程-22</t>
+    <t>Jmeter性能测试实战-P140</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>HTML、JavaScript复习</t>
+    <t>Jmeter性能测试实战-P210</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Vue2入门</t>
+    <t>凤凰项目-P140</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>工作习得</t>
+    <t>凤凰项目-P210</t>
+  </si>
+  <si>
+    <t>凤凰项目-P280</t>
+  </si>
+  <si>
+    <t>凤凰项目-P350</t>
+  </si>
+  <si>
+    <t>凤凰项目-P420</t>
+  </si>
+  <si>
+    <t>用户故事实战-P70</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>技能1</t>
+    <t>用户故事实战-P140</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>技能2</t>
+    <t>用户故事实战-P210</t>
+  </si>
+  <si>
+    <t>C课程-15</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>尚硅谷VUE核心技术视频</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A课程-38</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>逻辑英语系统4班180天</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C课程-38</t>
-  </si>
-  <si>
-    <t>C课程-40</t>
-  </si>
-  <si>
-    <t>E课程-02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E课程-08</t>
-  </si>
-  <si>
-    <t>E课程-10</t>
-  </si>
-  <si>
-    <t>E课程-04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E课程-12</t>
-  </si>
-  <si>
-    <t>E课程-14</t>
-  </si>
-  <si>
-    <t>E课程-16</t>
-  </si>
-  <si>
-    <t>E课程-18</t>
-  </si>
-  <si>
-    <t>E课程-20</t>
-  </si>
-  <si>
-    <t>E课程-22</t>
-  </si>
-  <si>
-    <t>E课程-24</t>
-  </si>
-  <si>
-    <t>E课程-26</t>
-  </si>
-  <si>
-    <t>E课程-28</t>
-  </si>
-  <si>
-    <t>E课程-30</t>
-  </si>
-  <si>
-    <t>E课程-32</t>
-  </si>
-  <si>
-    <t>E课程-34</t>
-  </si>
-  <si>
-    <t>E课程-36</t>
-  </si>
-  <si>
-    <t>E课程-38</t>
-  </si>
-  <si>
-    <t>E课程-40</t>
-  </si>
-  <si>
-    <t>D课程-02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D课程-04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D课程-06</t>
-  </si>
-  <si>
-    <t>D课程-08</t>
-  </si>
-  <si>
-    <t>D课程-10</t>
-  </si>
-  <si>
-    <t>D课程-12</t>
-  </si>
-  <si>
-    <t>D课程-14</t>
-  </si>
-  <si>
-    <t>D课程-16</t>
-  </si>
-  <si>
-    <t>D课程-18</t>
-  </si>
-  <si>
-    <t>D课程-20</t>
-  </si>
-  <si>
-    <t>D课程-22</t>
-  </si>
-  <si>
-    <t>D课程-24</t>
-  </si>
-  <si>
-    <t>D课程-26</t>
-  </si>
-  <si>
-    <t>D课程-28</t>
-  </si>
-  <si>
-    <t>D课程-30</t>
-  </si>
-  <si>
-    <t>D课程-32</t>
-  </si>
-  <si>
-    <t>D课程-34</t>
-  </si>
-  <si>
-    <t>D课程-36</t>
-  </si>
-  <si>
-    <t>D课程-38</t>
-  </si>
-  <si>
-    <t>D课程-40</t>
-  </si>
-  <si>
-    <t>B课程-02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B课程-06</t>
-  </si>
-  <si>
-    <t>B课程-04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B课程-08</t>
-  </si>
-  <si>
-    <t>B课程-10</t>
-  </si>
-  <si>
-    <t>B课程-12</t>
-  </si>
-  <si>
-    <t>春节放假</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B课程-14</t>
-  </si>
-  <si>
-    <t>B课程-16</t>
-  </si>
-  <si>
-    <t>B课程-18</t>
-  </si>
-  <si>
-    <t>B课程-20</t>
-  </si>
-  <si>
-    <t>B课程-22</t>
-  </si>
-  <si>
-    <t>B课程-24</t>
-  </si>
-  <si>
-    <t>B课程-26</t>
-  </si>
-  <si>
-    <t>B课程-28</t>
-  </si>
-  <si>
-    <t>B课程-30</t>
-  </si>
-  <si>
-    <t>B课程-32</t>
-  </si>
-  <si>
-    <t>B课程-34</t>
-  </si>
-  <si>
-    <t>B课程-36</t>
-  </si>
-  <si>
-    <t>B课程-38</t>
-  </si>
-  <si>
-    <t>B课程-40</t>
-  </si>
-  <si>
-    <t>C课程-14</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C课程-05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TypeScript入门</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C课程-06</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>性能测试</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E课程-06</t>
+    <t>C课程-16</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2057,13 +2223,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4567,16 +4748,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>76199</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>419101</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>476251</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4610,16 +4791,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4948,8 +5129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7853CF4-801B-49FD-A980-140083D542D0}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4978,7 +5159,7 @@
       </c>
       <c r="F1" s="20"/>
       <c r="G1" s="18" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="17" t="s">
@@ -5009,10 +5190,10 @@
         <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
@@ -5644,7 +5825,7 @@
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I28" s="4">
         <v>52</v>
@@ -5653,7 +5834,7 @@
         <v>48</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -5669,7 +5850,7 @@
         <v>43</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G29" s="3"/>
       <c r="I29" s="4">
@@ -5679,7 +5860,7 @@
         <v>49</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -5695,7 +5876,7 @@
         <v>44</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -5706,7 +5887,7 @@
         <v>49</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -5722,7 +5903,7 @@
         <v>45</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -5733,7 +5914,7 @@
         <v>49</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -5749,10 +5930,10 @@
         <v>46</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="4">
@@ -5762,7 +5943,7 @@
         <v>49</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -5778,10 +5959,10 @@
         <v>47</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="4">
@@ -5791,7 +5972,7 @@
         <v>51</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -5807,10 +5988,10 @@
         <v>48</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="4">
@@ -5834,10 +6015,10 @@
         <v>49</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="4">
@@ -5861,10 +6042,10 @@
         <v>50</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="4">
@@ -5888,10 +6069,10 @@
         <v>51</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="4">
@@ -5915,10 +6096,10 @@
         <v>52</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="4">
@@ -5928,7 +6109,7 @@
         <v>65</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -5944,10 +6125,10 @@
         <v>53</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="4">
@@ -5971,10 +6152,10 @@
         <v>54</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="4">
@@ -5995,13 +6176,13 @@
         <v>81</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="4">
@@ -6011,7 +6192,7 @@
         <v>65</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -6027,10 +6208,10 @@
         <v>55</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="4">
@@ -6054,10 +6235,10 @@
         <v>56</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="4">
@@ -6081,10 +6262,10 @@
         <v>57</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="4">
@@ -6094,7 +6275,7 @@
         <v>68</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -6103,17 +6284,17 @@
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="7" t="s">
-        <v>85</v>
+        <v>179</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="4">
@@ -6137,10 +6318,10 @@
         <v>59</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="4">
@@ -6164,10 +6345,10 @@
         <v>60</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="4">
@@ -6191,7 +6372,7 @@
         <v>61</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -6216,7 +6397,7 @@
         <v>62</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -6241,7 +6422,7 @@
         <v>63</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -6266,7 +6447,7 @@
         <v>64</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -6289,7 +6470,7 @@
         <v>65</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -6299,7 +6480,9 @@
       <c r="J52" s="4">
         <v>72</v>
       </c>
-      <c r="K52" s="3"/>
+      <c r="K52" s="3" t="s">
+        <v>195</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -6321,26 +6504,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B5DF0C-4498-4702-842C-511FF1DC7909}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="4" max="4" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="30.375" customWidth="1"/>
+    <col min="3" max="3" width="23.375" customWidth="1"/>
+    <col min="4" max="4" width="19.875" customWidth="1"/>
     <col min="5" max="5" width="12.875" customWidth="1"/>
     <col min="6" max="6" width="21.375" customWidth="1"/>
     <col min="7" max="7" width="16.125" customWidth="1"/>
-    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="29.125" customWidth="1"/>
     <col min="9" max="10" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -6363,17 +6546,20 @@
       <c r="J1" s="17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="17"/>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>173</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>174</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
@@ -6382,28 +6568,26 @@
         <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>172</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="17"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>44199</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="3"/>
+      <c r="B3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>64</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -6411,23 +6595,22 @@
         <v>2</v>
       </c>
       <c r="J3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>44206</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>93</v>
-      </c>
+      <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="8" t="s">
         <v>65</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6435,23 +6618,22 @@
         <v>4</v>
       </c>
       <c r="J4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>44213</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>94</v>
-      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>106</v>
+      <c r="E5" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -6459,219 +6641,275 @@
         <v>6</v>
       </c>
       <c r="J5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>44220</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>107</v>
+      <c r="E6" s="8" t="s">
+        <v>104</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="4">
         <v>8</v>
       </c>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J6" s="4">
+        <v>4</v>
+      </c>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>44227</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>108</v>
+      <c r="E7" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="4">
         <v>10</v>
       </c>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J7" s="4">
+        <v>6</v>
+      </c>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>44234</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F8" s="3"/>
+      <c r="E8" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="4">
         <v>12</v>
       </c>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J8" s="4">
+        <v>6</v>
+      </c>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
         <v>44241</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I9" s="13">
         <v>14</v>
       </c>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J9" s="4">
+        <v>6</v>
+      </c>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <v>44248</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I10" s="13">
         <v>14</v>
       </c>
-      <c r="J10" s="13"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J10" s="4">
+        <v>6</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>44255</v>
       </c>
+      <c r="C11" s="3" t="s">
+        <v>184</v>
+      </c>
       <c r="E11" s="3" t="s">
-        <v>173</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="H11" s="3"/>
       <c r="I11" s="4">
         <v>14</v>
       </c>
       <c r="J11" s="14"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>44262</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>185</v>
+      </c>
       <c r="D12" s="3"/>
       <c r="E12" t="s">
-        <v>109</v>
-      </c>
-      <c r="F12" s="3"/>
+        <v>106</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="4">
         <v>16</v>
       </c>
       <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>44269</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>186</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" t="s">
-        <v>110</v>
-      </c>
-      <c r="F13" s="3"/>
+        <v>107</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="4">
         <v>18</v>
       </c>
       <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>44276</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>183</v>
+      </c>
       <c r="E14" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14" s="3"/>
+        <v>109</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="4">
         <v>20</v>
       </c>
       <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>44283</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="E15" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="I15" s="4">
         <v>22</v>
       </c>
       <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>44290</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="E16" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -6679,358 +6917,461 @@
         <v>24</v>
       </c>
       <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>44297</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>189</v>
+      </c>
       <c r="E17" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F17" s="3"/>
+        <v>112</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
       <c r="I17" s="4">
         <v>26</v>
       </c>
       <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>44304</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>190</v>
+      </c>
       <c r="E18" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F18" s="3"/>
+        <v>113</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="4">
         <v>28</v>
       </c>
       <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>44311</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>191</v>
+      </c>
       <c r="E19" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F19" s="3"/>
+        <v>114</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="I19" s="4">
         <v>30</v>
       </c>
       <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>44318</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>192</v>
+      </c>
       <c r="E20" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F20" s="3"/>
+        <v>115</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="4">
         <v>32</v>
       </c>
       <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>44325</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>193</v>
+      </c>
       <c r="E21" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F21" s="3"/>
+        <v>116</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="4">
         <v>34</v>
       </c>
       <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>44332</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>194</v>
+      </c>
       <c r="E22" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F22" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="4">
         <v>36</v>
       </c>
       <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>44339</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F23" s="3"/>
+        <v>118</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="H23" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="I23" s="4">
         <v>38</v>
       </c>
       <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>44346</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="F24" s="3"/>
+        <v>119</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="4">
         <v>40</v>
       </c>
       <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>44353</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F25" s="3"/>
+        <v>120</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="4">
         <v>42</v>
       </c>
       <c r="J25" s="4"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>44360</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F26" s="3"/>
+        <v>121</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="4">
         <v>44</v>
       </c>
       <c r="J26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>44367</v>
       </c>
-      <c r="B27" s="3"/>
+      <c r="B27" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F27" s="3"/>
+        <v>122</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="H27" s="3" t="s">
+        <v>178</v>
+      </c>
       <c r="I27" s="4">
         <v>46</v>
       </c>
       <c r="J27" s="4"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>44374</v>
       </c>
-      <c r="B28" s="3"/>
+      <c r="B28" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="F28" s="3"/>
+        <v>123</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="4">
         <v>48</v>
       </c>
       <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>44381</v>
       </c>
-      <c r="B29" s="3"/>
+      <c r="B29" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F29" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="4">
         <v>50</v>
       </c>
       <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>44388</v>
       </c>
-      <c r="B30" s="3"/>
+      <c r="B30" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F30" s="3"/>
+        <v>125</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="4">
         <v>52</v>
       </c>
       <c r="J30" s="4"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>44395</v>
       </c>
-      <c r="B31" s="3"/>
+      <c r="B31" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F31" s="3"/>
+        <v>126</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="4">
         <v>54</v>
       </c>
       <c r="J31" s="4"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>44402</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F32" s="3"/>
+        <v>127</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="4">
         <v>56</v>
       </c>
       <c r="J32" s="4"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>44409</v>
       </c>
-      <c r="B33" s="3"/>
+      <c r="B33" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F33" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="4">
         <v>58</v>
       </c>
       <c r="J33" s="4"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>44416</v>
       </c>
-      <c r="B34" s="3"/>
+      <c r="B34" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F34" s="3"/>
+        <v>129</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="4">
         <v>60</v>
       </c>
       <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>44423</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="7" t="s">
+        <v>179</v>
+      </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F35" s="3"/>
+        <v>130</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="4">
         <v>62</v>
       </c>
       <c r="J35" s="4"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>44430</v>
       </c>
-      <c r="B36" s="3"/>
+      <c r="B36" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -7039,16 +7380,19 @@
         <v>64</v>
       </c>
       <c r="J36" s="4"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>44437</v>
       </c>
-      <c r="B37" s="3"/>
+      <c r="B37" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -7057,16 +7401,19 @@
         <v>66</v>
       </c>
       <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>44444</v>
       </c>
-      <c r="B38" s="3"/>
+      <c r="B38" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -7075,16 +7422,19 @@
         <v>68</v>
       </c>
       <c r="J38" s="4"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>44451</v>
       </c>
-      <c r="B39" s="3"/>
+      <c r="B39" s="7" t="s">
+        <v>87</v>
+      </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -7093,16 +7443,19 @@
         <v>70</v>
       </c>
       <c r="J39" s="4"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>44458</v>
       </c>
-      <c r="B40" s="3"/>
+      <c r="B40" s="7" t="s">
+        <v>87</v>
+      </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
@@ -7111,16 +7464,19 @@
         <v>72</v>
       </c>
       <c r="J40" s="4"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>44465</v>
       </c>
-      <c r="B41" s="3"/>
+      <c r="B41" s="7" t="s">
+        <v>87</v>
+      </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
@@ -7129,8 +7485,9 @@
         <v>74</v>
       </c>
       <c r="J41" s="4"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>44472</v>
       </c>
@@ -7138,7 +7495,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -7147,8 +7504,9 @@
         <v>76</v>
       </c>
       <c r="J42" s="4"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42" s="3"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>44479</v>
       </c>
@@ -7156,7 +7514,7 @@
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
@@ -7165,16 +7523,19 @@
         <v>78</v>
       </c>
       <c r="J43" s="4"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>44486</v>
       </c>
-      <c r="B44" s="3"/>
+      <c r="B44" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -7183,16 +7544,19 @@
         <v>80</v>
       </c>
       <c r="J44" s="4"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>44493</v>
       </c>
-      <c r="B45" s="3"/>
+      <c r="B45" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -7201,16 +7565,19 @@
         <v>82</v>
       </c>
       <c r="J45" s="4"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>44500</v>
       </c>
-      <c r="B46" s="3"/>
+      <c r="B46" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -7219,16 +7586,19 @@
         <v>84</v>
       </c>
       <c r="J46" s="4"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>44507</v>
       </c>
-      <c r="B47" s="3"/>
+      <c r="B47" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -7237,16 +7607,19 @@
         <v>86</v>
       </c>
       <c r="J47" s="4"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>44514</v>
       </c>
-      <c r="B48" s="3"/>
+      <c r="B48" s="8" t="s">
+        <v>78</v>
+      </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -7255,16 +7628,19 @@
         <v>88</v>
       </c>
       <c r="J48" s="4"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>44521</v>
       </c>
-      <c r="B49" s="3"/>
+      <c r="B49" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -7273,16 +7649,19 @@
         <v>90</v>
       </c>
       <c r="J49" s="4"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>44528</v>
       </c>
-      <c r="B50" s="3"/>
+      <c r="B50" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -7291,16 +7670,19 @@
         <v>92</v>
       </c>
       <c r="J50" s="4"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50" s="3"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>44535</v>
       </c>
-      <c r="B51" s="3"/>
+      <c r="B51" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -7309,16 +7691,19 @@
         <v>94</v>
       </c>
       <c r="J51" s="4"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>44542</v>
       </c>
-      <c r="B52" s="3"/>
+      <c r="B52" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
@@ -7327,16 +7712,19 @@
         <v>96</v>
       </c>
       <c r="J52" s="4"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>44549</v>
       </c>
-      <c r="B53" s="3"/>
+      <c r="B53" s="8" t="s">
+        <v>83</v>
+      </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
@@ -7345,16 +7733,19 @@
         <v>98</v>
       </c>
       <c r="J53" s="4"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K53" s="3"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>44556</v>
       </c>
-      <c r="B54" s="3"/>
+      <c r="B54" s="8" t="s">
+        <v>84</v>
+      </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -7363,9 +7754,11 @@
         <v>100</v>
       </c>
       <c r="J54" s="4"/>
+      <c r="K54" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="K1:K2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
@@ -7383,10 +7776,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2BC602-925C-49AB-BC80-18E4DF2512B1}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7402,7 +7795,7 @@
     <col min="9" max="10" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -7425,8 +7818,11 @@
       <c r="J1" s="17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="17"/>
       <c r="B2" s="9" t="s">
         <v>6</v>
@@ -7451,8 +7847,9 @@
       </c>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="17"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>44563</v>
       </c>
@@ -7460,11 +7857,9 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>105</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="4">
@@ -7473,8 +7868,9 @@
       <c r="J3" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>44570</v>
       </c>
@@ -7482,11 +7878,9 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>105</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="4">
@@ -7495,8 +7889,9 @@
       <c r="J4" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>44577</v>
       </c>
@@ -7504,11 +7899,9 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>105</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="4">
@@ -7517,8 +7910,9 @@
       <c r="J5" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>44584</v>
       </c>
@@ -7526,19 +7920,18 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>105</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="4">
         <v>8</v>
       </c>
       <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>44591</v>
       </c>
@@ -7546,79 +7939,80 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>105</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="4">
         <v>10</v>
       </c>
       <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="16">
         <v>44598</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I8" s="4">
         <v>10</v>
       </c>
       <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="16">
         <v>44605</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I9" s="4">
         <v>10</v>
       </c>
       <c r="J9" s="13"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>44612</v>
       </c>
@@ -7626,7 +8020,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -7635,8 +8029,9 @@
         <v>12</v>
       </c>
       <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>44619</v>
       </c>
@@ -7644,7 +8039,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -7653,8 +8048,9 @@
         <v>14</v>
       </c>
       <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>44626</v>
       </c>
@@ -7662,7 +8058,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -7671,8 +8067,9 @@
         <v>16</v>
       </c>
       <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>44633</v>
       </c>
@@ -7680,7 +8077,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -7689,8 +8086,9 @@
         <v>18</v>
       </c>
       <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>44640</v>
       </c>
@@ -7698,7 +8096,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -7707,8 +8105,9 @@
         <v>20</v>
       </c>
       <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>44647</v>
       </c>
@@ -7716,7 +8115,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -7724,8 +8123,9 @@
         <v>22</v>
       </c>
       <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>44654</v>
       </c>
@@ -7733,7 +8133,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -7741,8 +8141,9 @@
         <v>24</v>
       </c>
       <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>44661</v>
       </c>
@@ -7750,7 +8151,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -7759,8 +8160,9 @@
         <v>26</v>
       </c>
       <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>44668</v>
       </c>
@@ -7768,7 +8170,7 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -7777,8 +8179,9 @@
         <v>28</v>
       </c>
       <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>44675</v>
       </c>
@@ -7786,7 +8189,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -7795,8 +8198,9 @@
         <v>30</v>
       </c>
       <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>44682</v>
       </c>
@@ -7804,7 +8208,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -7813,8 +8217,9 @@
         <v>32</v>
       </c>
       <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>44689</v>
       </c>
@@ -7822,7 +8227,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -7831,8 +8236,9 @@
         <v>34</v>
       </c>
       <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>44696</v>
       </c>
@@ -7840,7 +8246,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -7849,8 +8255,9 @@
         <v>36</v>
       </c>
       <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>44703</v>
       </c>
@@ -7865,8 +8272,9 @@
         <v>38</v>
       </c>
       <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>44710</v>
       </c>
@@ -7881,8 +8289,9 @@
         <v>40</v>
       </c>
       <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>44717</v>
       </c>
@@ -7897,8 +8306,9 @@
         <v>42</v>
       </c>
       <c r="J25" s="4"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>44724</v>
       </c>
@@ -7913,8 +8323,9 @@
         <v>44</v>
       </c>
       <c r="J26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>44731</v>
       </c>
@@ -7929,8 +8340,9 @@
         <v>46</v>
       </c>
       <c r="J27" s="4"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>44738</v>
       </c>
@@ -7945,8 +8357,9 @@
         <v>48</v>
       </c>
       <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>44745</v>
       </c>
@@ -7961,8 +8374,9 @@
         <v>50</v>
       </c>
       <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>44752</v>
       </c>
@@ -7977,8 +8391,9 @@
         <v>52</v>
       </c>
       <c r="J30" s="4"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>44759</v>
       </c>
@@ -7993,8 +8408,9 @@
         <v>54</v>
       </c>
       <c r="J31" s="4"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>44766</v>
       </c>
@@ -8009,8 +8425,9 @@
         <v>56</v>
       </c>
       <c r="J32" s="4"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>44773</v>
       </c>
@@ -8025,8 +8442,9 @@
         <v>58</v>
       </c>
       <c r="J33" s="4"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>44780</v>
       </c>
@@ -8041,8 +8459,9 @@
         <v>60</v>
       </c>
       <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>44787</v>
       </c>
@@ -8057,8 +8476,9 @@
         <v>62</v>
       </c>
       <c r="J35" s="4"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>44794</v>
       </c>
@@ -8073,8 +8493,9 @@
         <v>64</v>
       </c>
       <c r="J36" s="4"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>44801</v>
       </c>
@@ -8089,8 +8510,9 @@
         <v>66</v>
       </c>
       <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>44808</v>
       </c>
@@ -8105,8 +8527,9 @@
         <v>68</v>
       </c>
       <c r="J38" s="4"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>44815</v>
       </c>
@@ -8121,8 +8544,9 @@
         <v>70</v>
       </c>
       <c r="J39" s="4"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>44822</v>
       </c>
@@ -8137,8 +8561,9 @@
         <v>72</v>
       </c>
       <c r="J40" s="4"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>44829</v>
       </c>
@@ -8153,8 +8578,9 @@
         <v>74</v>
       </c>
       <c r="J41" s="4"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>44836</v>
       </c>
@@ -8169,8 +8595,9 @@
         <v>76</v>
       </c>
       <c r="J42" s="4"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42" s="3"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>44843</v>
       </c>
@@ -8185,8 +8612,9 @@
         <v>78</v>
       </c>
       <c r="J43" s="4"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>44850</v>
       </c>
@@ -8201,8 +8629,9 @@
         <v>80</v>
       </c>
       <c r="J44" s="4"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>44857</v>
       </c>
@@ -8217,8 +8646,9 @@
         <v>82</v>
       </c>
       <c r="J45" s="4"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>44864</v>
       </c>
@@ -8233,8 +8663,9 @@
         <v>84</v>
       </c>
       <c r="J46" s="4"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>44871</v>
       </c>
@@ -8249,8 +8680,9 @@
         <v>86</v>
       </c>
       <c r="J47" s="4"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>44878</v>
       </c>
@@ -8265,8 +8697,9 @@
         <v>88</v>
       </c>
       <c r="J48" s="4"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>44885</v>
       </c>
@@ -8281,8 +8714,9 @@
         <v>90</v>
       </c>
       <c r="J49" s="4"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>44892</v>
       </c>
@@ -8297,8 +8731,9 @@
         <v>92</v>
       </c>
       <c r="J50" s="4"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50" s="3"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>44899</v>
       </c>
@@ -8313,8 +8748,9 @@
         <v>94</v>
       </c>
       <c r="J51" s="4"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>44906</v>
       </c>
@@ -8329,8 +8765,9 @@
         <v>96</v>
       </c>
       <c r="J52" s="4"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>44913</v>
       </c>
@@ -8345,8 +8782,9 @@
         <v>98</v>
       </c>
       <c r="J53" s="4"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K53" s="3"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>44920</v>
       </c>
@@ -8361,9 +8799,11 @@
         <v>100</v>
       </c>
       <c r="J54" s="4"/>
+      <c r="K54" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="K1:K2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>

</xml_diff>

<commit_message>
update course in march
</commit_message>
<xml_diff>
--- a/Personal/MillerToDoList.xlsx
+++ b/Personal/MillerToDoList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\notes\Personal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6764F0-9AC2-42C0-86A0-1386C99CDFCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BDF4E9-091A-450E-8EA7-416C461F8EC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17535" activeTab="1" xr2:uid="{FBB7AB9A-5833-4D53-A287-E17DA39A5383}"/>
   </bookViews>
@@ -1080,7 +1080,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1121,9 +1121,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2245,6 +2242,12 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5146,34 +5149,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="18" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="18" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="17" t="s">
+      <c r="H1" s="19"/>
+      <c r="I1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="16" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
@@ -5195,9 +5198,9 @@
       <c r="H2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
@@ -6507,7 +6510,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6524,34 +6527,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="18" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="18" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="17" t="s">
+      <c r="H1" s="19"/>
+      <c r="I1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="16" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="2" t="s">
         <v>173</v>
       </c>
@@ -6573,9 +6576,9 @@
       <c r="H2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
@@ -6715,7 +6718,7 @@
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="15">
+      <c r="A9" s="14">
         <v>44241</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -6748,7 +6751,7 @@
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="15">
+      <c r="A10" s="14">
         <v>44248</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -6799,7 +6802,9 @@
       <c r="I11" s="4">
         <v>14</v>
       </c>
-      <c r="J11" s="14"/>
+      <c r="J11" s="4">
+        <v>8</v>
+      </c>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -6822,7 +6827,9 @@
       <c r="I12" s="4">
         <v>16</v>
       </c>
-      <c r="J12" s="4"/>
+      <c r="J12" s="4">
+        <v>10</v>
+      </c>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -7796,34 +7803,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="18" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="18" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="17" t="s">
+      <c r="H1" s="19"/>
+      <c r="I1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="16" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
@@ -7845,9 +7852,9 @@
       <c r="H2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
@@ -7951,7 +7958,7 @@
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="16">
+      <c r="A8" s="15">
         <v>44598</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -7982,7 +7989,7 @@
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="16">
+      <c r="A9" s="15">
         <v>44605</v>
       </c>
       <c r="B9" s="12" t="s">

</xml_diff>